<commit_message>
Here we go again with the refactoring...but we learn.
</commit_message>
<xml_diff>
--- a/WorkBot/refactor/data/orders/UNFI/CompletedOrders/UNFI_Bakery_2025-09-03.xlsx
+++ b/WorkBot/refactor/data/orders/UNFI/CompletedOrders/UNFI_Bakery_2025-09-03.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,6 +475,708 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>267463-8</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Poppi Soda - Ginger Lime</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>24.07</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>24.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>272451-6</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Poppi Soda - Doc Pop</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>24.07</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>24.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>289451-7</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Just Tea - Peach</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>25.92</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>155.52</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>289450-9</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Just Tea - Original Green</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>25.92</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>25.92</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>289449-1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Just Tea - Moroccan Mint</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>25.92</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>77.76</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>289446-7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Just Tea - Berry Hibiscus</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>25.92</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>77.76</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>289448-3</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Just Tea - Honey green</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>25.92</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>103.68</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>289447-5</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Just Tea - Half &amp; Half</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>25.92</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>77.76</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1513555</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>San Pellegrino - Sparkling Water (750ml)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>28.61</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>28.61</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>280251-0</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>San Pellegrino - Aranciata Rossa (Blood Orange)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>26.94</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>26.94</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2802668</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>San Pellegrino - Melograno &amp; Arancia (Pomegranate)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>26.94</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>26.94</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>030570-6</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Martinelli's Apple Juice Squat</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>43.85</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>43.85</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>117597-5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>That's It - Apple &amp; Mango (Fruit Bar)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>18.18</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>18.18</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1551282</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>That's It - Apple &amp; Strawberry (Fruit Bar)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>16.24</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>16.24</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>112599-6</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Kind - Madagascar Vanilla Almond</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>21.86</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>21.86</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>285865-2</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Kind Bar - Dark Chocolate Cherry Cashew</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>21.86</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>21.86</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>236948-6</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Bob's Bar - Oat, PB Coconut</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>15.73</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>15.73</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>0647743</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Justin's - Peanut Butter Cup (Dk Choc)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>23.03</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>46.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>0695312</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Chocolove - Dk Choc Chilies &amp; Cherries</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>41.30</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>41.30</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>0193292</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Chocolove - Dk Choc Coffee Crunch</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>41.30</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>41.30</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>032727-0</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Tofutti - Plain (8oz)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>51.62</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>51.62</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2273316</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>GTS, Kombucha - Gingerade</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>42.02</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>42.02</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>110982-6</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Harmless Harvest - Coconut Water</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>65.48</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>65.48</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>223893-9</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Remedy - Superseed Fuel</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>25.06</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>75.18</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>223894-7</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Remedy - Matcha Fuel</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>25.06</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>25.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>223791-5</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Remedy - Drk Cacoa Essential</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>25.06</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>25.06</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>